<commit_message>
creat xml file script update
</commit_message>
<xml_diff>
--- a/Exam143Score.xlsx
+++ b/Exam143Score.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:I1048576"/>
@@ -487,6 +487,16 @@
           <t>2023/02/18_2</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>2023/02/18</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>2023/02/21</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -518,6 +528,12 @@
       <c r="I2" t="n">
         <v>0.375</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -549,6 +565,12 @@
       <c r="I3" t="n">
         <v>0.75</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -580,6 +602,12 @@
       <c r="I4" t="n">
         <v>0.7</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -611,6 +639,12 @@
       <c r="I5" t="n">
         <v>0.5</v>
       </c>
+      <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -642,6 +676,12 @@
       <c r="I6" t="n">
         <v>0.5</v>
       </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -673,6 +713,12 @@
       <c r="I7" t="n">
         <v>0.45</v>
       </c>
+      <c r="J7" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -704,6 +750,12 @@
       <c r="I8" t="n">
         <v>0.5</v>
       </c>
+      <c r="J8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -735,6 +787,12 @@
       <c r="I9" t="n">
         <v>0.625</v>
       </c>
+      <c r="J9" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -766,6 +824,12 @@
       <c r="I10" t="n">
         <v>0.875</v>
       </c>
+      <c r="J10" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -797,6 +861,12 @@
       <c r="I11" t="n">
         <v>0.7</v>
       </c>
+      <c r="J11" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.575</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -828,6 +898,12 @@
       <c r="I12" t="n">
         <v>0.45</v>
       </c>
+      <c r="J12" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -859,6 +935,12 @@
       <c r="I13" t="n">
         <v>0.825</v>
       </c>
+      <c r="J13" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -890,6 +972,12 @@
       <c r="I14" t="n">
         <v>0.7</v>
       </c>
+      <c r="J14" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -921,6 +1009,12 @@
       <c r="I15" t="n">
         <v>0.375</v>
       </c>
+      <c r="J15" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -952,6 +1046,12 @@
       <c r="I16" t="n">
         <v>0.575</v>
       </c>
+      <c r="J16" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -983,6 +1083,12 @@
       <c r="I17" t="n">
         <v>0</v>
       </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1014,6 +1120,12 @@
       <c r="I18" t="n">
         <v>0.7</v>
       </c>
+      <c r="J18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1045,6 +1157,12 @@
       <c r="I19" t="n">
         <v>0.875</v>
       </c>
+      <c r="J19" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1076,6 +1194,12 @@
       <c r="I20" t="n">
         <v>0.5</v>
       </c>
+      <c r="J20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1107,6 +1231,12 @@
       <c r="I21" t="n">
         <v>0.575</v>
       </c>
+      <c r="J21" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.575</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1138,6 +1268,12 @@
       <c r="I22" t="n">
         <v>0.7</v>
       </c>
+      <c r="J22" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1169,6 +1305,12 @@
       <c r="I23" t="n">
         <v>1</v>
       </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1200,6 +1342,12 @@
       <c r="I24" t="n">
         <v>0.5</v>
       </c>
+      <c r="J24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1231,6 +1379,12 @@
       <c r="I25" t="n">
         <v>0</v>
       </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1262,6 +1416,12 @@
       <c r="I26" t="n">
         <v>0.625</v>
       </c>
+      <c r="J26" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1293,6 +1453,12 @@
       <c r="I27" t="n">
         <v>0.7</v>
       </c>
+      <c r="J27" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1324,6 +1490,12 @@
       <c r="I28" t="n">
         <v>1.125</v>
       </c>
+      <c r="J28" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1355,6 +1527,12 @@
       <c r="I29" t="n">
         <v>0.575</v>
       </c>
+      <c r="J29" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1383,6 +1561,9 @@
       <c r="H30" t="n">
         <v>0.375</v>
       </c>
+      <c r="K30" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1414,6 +1595,12 @@
       <c r="I31" t="n">
         <v>0.5</v>
       </c>
+      <c r="J31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1445,6 +1632,12 @@
       <c r="I32" t="n">
         <v>0.625</v>
       </c>
+      <c r="J32" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1476,6 +1669,12 @@
       <c r="I33" t="n">
         <v>0.825</v>
       </c>
+      <c r="J33" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1507,6 +1706,12 @@
       <c r="I34" t="n">
         <v>0.625</v>
       </c>
+      <c r="J34" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1538,6 +1743,12 @@
       <c r="I35" t="n">
         <v>0.45</v>
       </c>
+      <c r="J35" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1569,6 +1780,12 @@
       <c r="I36" t="n">
         <v>0.75</v>
       </c>
+      <c r="J36" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1600,6 +1817,12 @@
       <c r="I37" t="n">
         <v>0.625</v>
       </c>
+      <c r="J37" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1631,6 +1854,12 @@
       <c r="I38" t="n">
         <v>1</v>
       </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.525</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -1662,6 +1891,12 @@
       <c r="I39" t="n">
         <v>0.45</v>
       </c>
+      <c r="J39" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -1693,6 +1928,12 @@
       <c r="I40" t="n">
         <v>0.575</v>
       </c>
+      <c r="J40" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -1724,6 +1965,12 @@
       <c r="I41" t="n">
         <v>0.325</v>
       </c>
+      <c r="J41" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1755,6 +2002,12 @@
       <c r="I42" t="n">
         <v>0.45</v>
       </c>
+      <c r="J42" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1786,6 +2039,12 @@
       <c r="I43" t="n">
         <v>0.625</v>
       </c>
+      <c r="J43" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1817,6 +2076,12 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1848,6 +2113,12 @@
       <c r="I45" t="n">
         <v>0.575</v>
       </c>
+      <c r="J45" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -1879,6 +2150,12 @@
       <c r="I46" t="n">
         <v>0.875</v>
       </c>
+      <c r="J46" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1910,6 +2187,12 @@
       <c r="I47" t="n">
         <v>0.75</v>
       </c>
+      <c r="J47" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1941,6 +2224,12 @@
       <c r="I48" t="n">
         <v>0.625</v>
       </c>
+      <c r="J48" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1972,6 +2261,12 @@
       <c r="I49" t="n">
         <v>0.25</v>
       </c>
+      <c r="J49" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -2003,6 +2298,12 @@
       <c r="I50" t="n">
         <v>0.7</v>
       </c>
+      <c r="J50" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -2034,6 +2335,12 @@
       <c r="I51" t="n">
         <v>1</v>
       </c>
+      <c r="J51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -2063,6 +2370,12 @@
         <v>0.575</v>
       </c>
       <c r="I52" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="K52" t="n">
         <v>0.825</v>
       </c>
     </row>
@@ -2618,7 +2931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DX53"/>
+  <dimension ref="A1:ED53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="DN1" workbookViewId="0">
       <selection activeCell="DS2" sqref="DS1:DX1048576"/>
@@ -2840,6 +3153,16 @@
           <t>2023/02/18_2</t>
         </is>
       </c>
+      <c r="DY1" s="14" t="inlineStr">
+        <is>
+          <t>2023/02/18</t>
+        </is>
+      </c>
+      <c r="EB1" s="14" t="inlineStr">
+        <is>
+          <t>2023/02/21</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3482,6 +3805,36 @@
           <t>成绩占比</t>
         </is>
       </c>
+      <c r="DY2" t="inlineStr">
+        <is>
+          <t>理论满分</t>
+        </is>
+      </c>
+      <c r="DZ2" t="inlineStr">
+        <is>
+          <t>原始成绩</t>
+        </is>
+      </c>
+      <c r="EA2" t="inlineStr">
+        <is>
+          <t>成绩占比</t>
+        </is>
+      </c>
+      <c r="EB2" t="inlineStr">
+        <is>
+          <t>理论满分</t>
+        </is>
+      </c>
+      <c r="EC2" t="inlineStr">
+        <is>
+          <t>原始成绩</t>
+        </is>
+      </c>
+      <c r="ED2" t="inlineStr">
+        <is>
+          <t>成绩占比</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3910,6 +4263,24 @@
       <c r="DX3" s="18" t="n">
         <v>0.375</v>
       </c>
+      <c r="DY3" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ3" s="18" t="n">
+        <v>15</v>
+      </c>
+      <c r="EA3" s="18" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="EB3" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC3" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="ED3" s="18" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4338,6 +4709,24 @@
       <c r="DX4" s="18" t="n">
         <v>0.75</v>
       </c>
+      <c r="DY4" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ4" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="EA4" s="18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="EB4" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC4" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED4" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4766,6 +5155,24 @@
       <c r="DX5" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY5" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ5" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA5" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB5" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC5" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED5" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5194,6 +5601,24 @@
       <c r="DX6" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY6" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ6" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA6" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB6" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC6" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="ED6" s="18" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5622,6 +6047,24 @@
       <c r="DX7" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY7" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ7" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA7" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB7" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC7" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED7" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6048,6 +6491,24 @@
         <v>18</v>
       </c>
       <c r="DX8" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="DY8" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ8" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="EA8" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="EB8" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC8" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="ED8" s="18" t="n">
         <v>0.45</v>
       </c>
     </row>
@@ -6476,6 +6937,24 @@
       <c r="DX9" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY9" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ9" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA9" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB9" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC9" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED9" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6904,6 +7383,24 @@
       <c r="DX10" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY10" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ10" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA10" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB10" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC10" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="ED10" s="18" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7332,6 +7829,24 @@
       <c r="DX11" s="18" t="n">
         <v>0.875</v>
       </c>
+      <c r="DY11" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ11" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="EA11" s="18" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="EB11" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC11" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED11" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7760,6 +8275,24 @@
       <c r="DX12" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY12" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ12" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA12" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB12" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC12" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="ED12" s="18" t="n">
+        <v>0.575</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8188,6 +8721,24 @@
       <c r="DX13" s="18" t="n">
         <v>0.45</v>
       </c>
+      <c r="DY13" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ13" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="EA13" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="EB13" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC13" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED13" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -8616,6 +9167,24 @@
       <c r="DX14" s="18" t="n">
         <v>0.825</v>
       </c>
+      <c r="DY14" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ14" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="EA14" s="18" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="EB14" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC14" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED14" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9044,6 +9613,24 @@
       <c r="DX15" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY15" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ15" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA15" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB15" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC15" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED15" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -9472,6 +10059,24 @@
       <c r="DX16" s="18" t="n">
         <v>0.375</v>
       </c>
+      <c r="DY16" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ16" s="18" t="n">
+        <v>15</v>
+      </c>
+      <c r="EA16" s="18" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="EB16" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED16" s="18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -9900,6 +10505,24 @@
       <c r="DX17" s="18" t="n">
         <v>0.575</v>
       </c>
+      <c r="DY17" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ17" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="EA17" s="18" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="EB17" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC17" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED17" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -10328,6 +10951,24 @@
       <c r="DX18" s="18" t="n">
         <v>0</v>
       </c>
+      <c r="DY18" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB18" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED18" s="18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -10756,6 +11397,24 @@
       <c r="DX19" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY19" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ19" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA19" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB19" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC19" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED19" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -11184,6 +11843,24 @@
       <c r="DX20" s="18" t="n">
         <v>0.875</v>
       </c>
+      <c r="DY20" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ20" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="EA20" s="18" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="EB20" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC20" s="18" t="n">
+        <v>15</v>
+      </c>
+      <c r="ED20" s="18" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -11612,6 +12289,24 @@
       <c r="DX21" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY21" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ21" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA21" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB21" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC21" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED21" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -12040,6 +12735,24 @@
       <c r="DX22" s="18" t="n">
         <v>0.575</v>
       </c>
+      <c r="DY22" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ22" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="EA22" s="18" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="EB22" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC22" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="ED22" s="18" t="n">
+        <v>0.575</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -12468,6 +13181,24 @@
       <c r="DX23" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY23" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ23" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA23" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB23" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC23" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED23" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -12896,6 +13627,24 @@
       <c r="DX24" s="18" t="n">
         <v>1</v>
       </c>
+      <c r="DY24" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ24" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EA24" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB24" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC24" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED24" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -13324,6 +14073,24 @@
       <c r="DX25" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY25" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ25" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA25" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB25" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC25" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED25" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -13752,6 +14519,24 @@
       <c r="DX26" s="18" t="n">
         <v>0</v>
       </c>
+      <c r="DY26" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ26" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA26" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB26" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC26" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="ED26" s="18" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -14180,6 +14965,24 @@
       <c r="DX27" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY27" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ27" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA27" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB27" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC27" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED27" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -14608,6 +15411,24 @@
       <c r="DX28" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY28" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ28" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA28" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB28" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC28" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="ED28" s="18" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -15036,6 +15857,24 @@
       <c r="DX29" s="18" t="n">
         <v>1.125</v>
       </c>
+      <c r="DY29" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ29" s="18" t="n">
+        <v>45</v>
+      </c>
+      <c r="EA29" s="18" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="EB29" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC29" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED29" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -15464,6 +16303,24 @@
       <c r="DX30" s="18" t="n">
         <v>0.575</v>
       </c>
+      <c r="DY30" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ30" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="EA30" s="18" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="EB30" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC30" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED30" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -15886,6 +16743,18 @@
       <c r="DV31" s="18" t="n">
         <v>40</v>
       </c>
+      <c r="DY31" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EB31" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC31" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="ED31" s="18" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -16314,6 +17183,24 @@
       <c r="DX32" s="18" t="n">
         <v>0.5</v>
       </c>
+      <c r="DY32" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ32" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="EA32" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="EB32" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC32" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED32" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -16742,6 +17629,24 @@
       <c r="DX33" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY33" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ33" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA33" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB33" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC33" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED33" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -17170,6 +18075,24 @@
       <c r="DX34" s="18" t="n">
         <v>0.825</v>
       </c>
+      <c r="DY34" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ34" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="EA34" s="18" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="EB34" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC34" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED34" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -17598,6 +18521,24 @@
       <c r="DX35" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY35" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ35" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA35" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB35" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC35" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED35" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -18026,6 +18967,24 @@
       <c r="DX36" s="18" t="n">
         <v>0.45</v>
       </c>
+      <c r="DY36" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ36" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="EA36" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="EB36" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC36" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED36" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -18454,6 +19413,24 @@
       <c r="DX37" s="18" t="n">
         <v>0.75</v>
       </c>
+      <c r="DY37" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ37" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="EA37" s="18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="EB37" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC37" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED37" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -18882,6 +19859,24 @@
       <c r="DX38" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY38" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ38" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA38" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB38" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC38" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED38" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -19310,6 +20305,24 @@
       <c r="DX39" s="18" t="n">
         <v>1</v>
       </c>
+      <c r="DY39" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ39" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EA39" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB39" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC39" s="18" t="n">
+        <v>21</v>
+      </c>
+      <c r="ED39" s="18" t="n">
+        <v>0.525</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -19738,6 +20751,24 @@
       <c r="DX40" s="18" t="n">
         <v>0.45</v>
       </c>
+      <c r="DY40" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ40" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="EA40" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="EB40" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC40" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED40" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -20166,6 +21197,24 @@
       <c r="DX41" s="18" t="n">
         <v>0.575</v>
       </c>
+      <c r="DY41" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ41" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="EA41" s="18" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="EB41" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC41" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="ED41" s="18" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -20594,6 +21643,24 @@
       <c r="DX42" s="18" t="n">
         <v>0.325</v>
       </c>
+      <c r="DY42" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ42" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="EA42" s="18" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="EB42" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC42" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED42" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -21022,6 +22089,24 @@
       <c r="DX43" s="18" t="n">
         <v>0.45</v>
       </c>
+      <c r="DY43" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ43" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="EA43" s="18" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="EB43" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC43" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED43" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -21450,6 +22535,24 @@
       <c r="DX44" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY44" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ44" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA44" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB44" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC44" s="18" t="n">
+        <v>38</v>
+      </c>
+      <c r="ED44" s="18" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -21878,6 +22981,24 @@
       <c r="DX45" s="18" t="n">
         <v>0</v>
       </c>
+      <c r="DY45" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ45" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA45" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB45" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC45" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED45" s="18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -22306,6 +23427,24 @@
       <c r="DX46" s="18" t="n">
         <v>0.575</v>
       </c>
+      <c r="DY46" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ46" s="18" t="n">
+        <v>23</v>
+      </c>
+      <c r="EA46" s="18" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="EB46" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC46" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED46" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -22734,6 +23873,24 @@
       <c r="DX47" s="18" t="n">
         <v>0.875</v>
       </c>
+      <c r="DY47" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ47" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="EA47" s="18" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="EB47" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC47" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED47" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -23162,6 +24319,24 @@
       <c r="DX48" s="18" t="n">
         <v>0.75</v>
       </c>
+      <c r="DY48" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ48" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="EA48" s="18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="EB48" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC48" s="18" t="n">
+        <v>35</v>
+      </c>
+      <c r="ED48" s="18" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -23590,6 +24765,24 @@
       <c r="DX49" s="18" t="n">
         <v>0.625</v>
       </c>
+      <c r="DY49" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ49" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="EA49" s="18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="EB49" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC49" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="ED49" s="18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -24018,6 +25211,24 @@
       <c r="DX50" s="18" t="n">
         <v>0.25</v>
       </c>
+      <c r="DY50" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ50" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="EA50" s="18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="EB50" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC50" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="ED50" s="18" t="n">
+        <v>0.775</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -24446,6 +25657,24 @@
       <c r="DX51" s="18" t="n">
         <v>0.7</v>
       </c>
+      <c r="DY51" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ51" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="EA51" s="18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="EB51" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC51" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="ED51" s="18" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -24874,6 +26103,24 @@
       <c r="DX52" s="18" t="n">
         <v>1</v>
       </c>
+      <c r="DY52" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ52" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EA52" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB52" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC52" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="ED52" s="18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -25302,9 +26549,27 @@
       <c r="DX53" s="18" t="n">
         <v>0.825</v>
       </c>
+      <c r="DY53" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="DZ53" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="EA53" s="18" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="EB53" s="18" t="n">
+        <v>40</v>
+      </c>
+      <c r="EC53" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="ED53" s="18" t="n">
+        <v>0.825</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="43">
     <mergeCell ref="U1:W1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -25346,6 +26611,8 @@
     <mergeCell ref="DG1:DI1"/>
     <mergeCell ref="DS1:DU1"/>
     <mergeCell ref="DV1:DX1"/>
+    <mergeCell ref="DY1:EA1"/>
+    <mergeCell ref="EB1:ED1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>